<commit_message>
Work on test coverage
</commit_message>
<xml_diff>
--- a/data/Visitors.xlsx
+++ b/data/Visitors.xlsx
@@ -96,10 +96,10 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
@@ -490,7 +490,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.8046875" defaultRowHeight="14.25" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.83984375" defaultRowHeight="14.25" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData/>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
@@ -506,64 +506,70 @@
   </sheetPr>
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.8046875" defaultRowHeight="14.25" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.83984375" defaultRowHeight="14.25" zeroHeight="0" outlineLevelRow="0"/>
+  <cols>
+    <col width="15.28" customWidth="1" style="7" min="1" max="1"/>
+    <col width="22.36" customWidth="1" style="7" min="2" max="2"/>
+    <col width="21.95" customWidth="1" style="7" min="3" max="3"/>
+    <col width="31.95" customWidth="1" style="7" min="4" max="4"/>
+  </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1" s="7">
-      <c r="A1" s="8" t="inlineStr">
+    <row r="1" ht="14.25" customHeight="1" s="8">
+      <c r="A1" s="7" t="inlineStr">
         <is>
           <t>A Number</t>
         </is>
       </c>
-      <c r="B1" s="8" t="inlineStr">
+      <c r="B1" s="7" t="inlineStr">
         <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="C1" s="8" t="inlineStr">
+      <c r="C1" s="7" t="inlineStr">
         <is>
           <t>Courses</t>
         </is>
       </c>
-      <c r="D1" s="8" t="inlineStr">
+      <c r="D1" s="7" t="inlineStr">
         <is>
           <t>Visit Dates</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="14.25" customHeight="1" s="7">
-      <c r="A2" s="8" t="inlineStr">
+    <row r="2" ht="14.25" customHeight="1" s="8">
+      <c r="A2" s="7" t="inlineStr">
         <is>
           <t>A00444555</t>
         </is>
       </c>
-      <c r="B2" s="8" t="inlineStr">
+      <c r="B2" s="7" t="inlineStr">
         <is>
           <t>Morgan Curry</t>
         </is>
       </c>
-      <c r="C2" s="8" t="inlineStr">
+      <c r="C2" s="7" t="inlineStr">
         <is>
           <t>1910:N35</t>
         </is>
       </c>
-      <c r="D2" s="8" t="inlineStr">
-        <is>
-          <t>06/25/2406/25/2406/27/24</t>
+      <c r="D2" s="7" t="inlineStr">
+        <is>
+          <t>03/08/2404/10/2404/17/24</t>
         </is>
       </c>
       <c r="E2" s="9" t="n"/>
     </row>
-    <row r="3" ht="14.25" customHeight="1" s="7">
-      <c r="A3" s="8" t="inlineStr">
+    <row r="3" ht="14.25" customHeight="1" s="8">
+      <c r="A3" s="7" t="inlineStr">
         <is>
           <t>A00404303</t>
         </is>
       </c>
-      <c r="B3" s="8" t="inlineStr">
+      <c r="B3" s="7" t="inlineStr">
         <is>
           <t>Elias Shaw</t>
         </is>
@@ -574,20 +580,20 @@
 </t>
         </is>
       </c>
-      <c r="D3" s="8" t="inlineStr">
-        <is>
-          <t>06/25/24</t>
+      <c r="D3" s="7" t="inlineStr">
+        <is>
+          <t>03/11/24</t>
         </is>
       </c>
       <c r="E3" s="9" t="n"/>
     </row>
-    <row r="4" ht="14.25" customHeight="1" s="7">
-      <c r="A4" s="8" t="inlineStr">
+    <row r="4" ht="14.25" customHeight="1" s="8">
+      <c r="A4" s="7" t="inlineStr">
         <is>
           <t>A00909111</t>
         </is>
       </c>
-      <c r="B4" s="8" t="inlineStr">
+      <c r="B4" s="7" t="inlineStr">
         <is>
           <t>Bruno Osborne</t>
         </is>
@@ -598,20 +604,20 @@
 </t>
         </is>
       </c>
-      <c r="D4" s="8" t="inlineStr">
-        <is>
-          <t>06/25/24</t>
+      <c r="D4" s="7" t="inlineStr">
+        <is>
+          <t>04/05/24</t>
         </is>
       </c>
       <c r="E4" s="9" t="n"/>
     </row>
-    <row r="5" ht="14.25" customHeight="1" s="7">
-      <c r="A5" s="8" t="inlineStr">
+    <row r="5" ht="14.25" customHeight="1" s="8">
+      <c r="A5" s="7" t="inlineStr">
         <is>
           <t>A00898989</t>
         </is>
       </c>
-      <c r="B5" s="8" t="inlineStr">
+      <c r="B5" s="7" t="inlineStr">
         <is>
           <t>Arely Barry</t>
         </is>
@@ -621,20 +627,20 @@
           <t>1710:N35</t>
         </is>
       </c>
-      <c r="D5" s="8" t="inlineStr">
-        <is>
-          <t>06/25/24</t>
+      <c r="D5" s="7" t="inlineStr">
+        <is>
+          <t>04/07/24</t>
         </is>
       </c>
       <c r="E5" s="9" t="n"/>
     </row>
-    <row r="6" ht="14.25" customHeight="1" s="7">
-      <c r="A6" s="8" t="inlineStr">
+    <row r="6" ht="14.25" customHeight="1" s="8">
+      <c r="A6" s="7" t="inlineStr">
         <is>
           <t>A00242424</t>
         </is>
       </c>
-      <c r="B6" s="8" t="inlineStr">
+      <c r="B6" s="7" t="inlineStr">
         <is>
           <t>Solomon Giles</t>
         </is>
@@ -644,43 +650,43 @@
           <t>2010:N30</t>
         </is>
       </c>
-      <c r="D6" s="8" t="inlineStr">
-        <is>
-          <t>06/25/2406/27/24</t>
+      <c r="D6" s="7" t="inlineStr">
+        <is>
+          <t>04/07/2404/10/24</t>
         </is>
       </c>
       <c r="E6" s="9" t="n"/>
     </row>
-    <row r="7" ht="14.25" customHeight="1" s="7">
-      <c r="A7" s="8" t="inlineStr">
+    <row r="7" ht="14.25" customHeight="1" s="8">
+      <c r="A7" s="7" t="inlineStr">
         <is>
           <t>A00123456</t>
         </is>
       </c>
-      <c r="B7" s="8" t="inlineStr">
+      <c r="B7" s="7" t="inlineStr">
         <is>
           <t>Finley Jones</t>
         </is>
       </c>
-      <c r="C7" s="8" t="inlineStr">
+      <c r="C7" s="7" t="inlineStr">
         <is>
           <t>2110:N30</t>
         </is>
       </c>
-      <c r="D7" s="8" t="inlineStr">
-        <is>
-          <t>06/25/24</t>
+      <c r="D7" s="7" t="inlineStr">
+        <is>
+          <t>04/15/24</t>
         </is>
       </c>
       <c r="E7" s="9" t="n"/>
     </row>
-    <row r="8" ht="14.25" customHeight="1" s="7">
-      <c r="A8" s="8" t="inlineStr">
+    <row r="8" ht="14.25" customHeight="1" s="8">
+      <c r="A8" s="7" t="inlineStr">
         <is>
           <t>A00654321</t>
         </is>
       </c>
-      <c r="B8" s="8" t="inlineStr">
+      <c r="B8" s="7" t="inlineStr">
         <is>
           <t>Jaxon Frederick</t>
         </is>
@@ -690,20 +696,20 @@
           <t>1910:N35</t>
         </is>
       </c>
-      <c r="D8" s="8" t="inlineStr">
-        <is>
-          <t>06/25/24</t>
+      <c r="D8" s="7" t="inlineStr">
+        <is>
+          <t>04/17/24</t>
         </is>
       </c>
       <c r="E8" s="9" t="n"/>
     </row>
-    <row r="9" ht="14.25" customHeight="1" s="7">
-      <c r="A9" s="8" t="inlineStr">
+    <row r="9" ht="14.25" customHeight="1" s="8">
+      <c r="A9" s="7" t="inlineStr">
         <is>
           <t>A00345345</t>
         </is>
       </c>
-      <c r="B9" s="8" t="inlineStr">
+      <c r="B9" s="7" t="inlineStr">
         <is>
           <t>Ari Stapler</t>
         </is>
@@ -713,19 +719,19 @@
           <t>1920:N30</t>
         </is>
       </c>
-      <c r="D9" s="8" t="inlineStr">
-        <is>
-          <t>06/27/24</t>
-        </is>
-      </c>
-    </row>
-    <row r="10" ht="14.25" customHeight="1" s="7">
-      <c r="A10" s="8" t="inlineStr">
+      <c r="D9" s="7" t="inlineStr">
+        <is>
+          <t>05/02/24</t>
+        </is>
+      </c>
+    </row>
+    <row r="10" ht="14.25" customHeight="1" s="8">
+      <c r="A10" s="7" t="inlineStr">
         <is>
           <t>A00456123</t>
         </is>
       </c>
-      <c r="B10" s="8" t="inlineStr">
+      <c r="B10" s="7" t="inlineStr">
         <is>
           <t>Selena Ramirez</t>
         </is>
@@ -735,19 +741,19 @@
           <t>1920:N30</t>
         </is>
       </c>
-      <c r="D10" s="8" t="inlineStr">
-        <is>
-          <t>06/27/24</t>
-        </is>
-      </c>
-    </row>
-    <row r="11" ht="14.25" customHeight="1" s="7">
-      <c r="A11" s="8" t="inlineStr">
+      <c r="D10" s="7" t="inlineStr">
+        <is>
+          <t>05/10/24</t>
+        </is>
+      </c>
+    </row>
+    <row r="11" ht="14.25" customHeight="1" s="8">
+      <c r="A11" s="7" t="inlineStr">
         <is>
           <t>A00999111</t>
         </is>
       </c>
-      <c r="B11" s="8" t="inlineStr">
+      <c r="B11" s="7" t="inlineStr">
         <is>
           <t>Britt Faff</t>
         </is>
@@ -757,19 +763,19 @@
           <t>1720:N35</t>
         </is>
       </c>
-      <c r="D11" s="8" t="inlineStr">
-        <is>
-          <t>06/28/2406/29/24</t>
-        </is>
-      </c>
-    </row>
-    <row r="12" ht="14.25" customHeight="1" s="7">
-      <c r="A12" s="8" t="inlineStr">
+      <c r="D11" s="7" t="inlineStr">
+        <is>
+          <t>05/16/2405/20/24</t>
+        </is>
+      </c>
+    </row>
+    <row r="12" ht="14.25" customHeight="1" s="8">
+      <c r="A12" s="7" t="inlineStr">
         <is>
           <t>A00663224</t>
         </is>
       </c>
-      <c r="B12" s="8" t="inlineStr">
+      <c r="B12" s="7" t="inlineStr">
         <is>
           <t>Denise Harlow</t>
         </is>
@@ -779,85 +785,60 @@
           <t>2110:N30</t>
         </is>
       </c>
-      <c r="D12" s="8" t="inlineStr">
-        <is>
-          <t>06/28/24</t>
-        </is>
-      </c>
-    </row>
-    <row r="13" ht="14.25" customHeight="1" s="7">
-      <c r="A13" s="8" t="n"/>
-      <c r="B13" s="8" t="n"/>
-      <c r="C13" s="10" t="n"/>
-      <c r="D13" s="8" t="n"/>
-    </row>
-    <row r="14" ht="14.25" customHeight="1" s="7">
-      <c r="A14" s="8" t="n"/>
-      <c r="B14" s="8" t="n"/>
-      <c r="C14" s="8" t="n"/>
-      <c r="D14" s="8" t="n"/>
-    </row>
-    <row r="15" ht="14.25" customHeight="1" s="7">
-      <c r="A15" s="8" t="n"/>
-      <c r="B15" s="8" t="n"/>
-      <c r="C15" s="8" t="n"/>
-      <c r="D15" s="8" t="n"/>
-    </row>
-    <row r="16" ht="14.25" customHeight="1" s="7">
-      <c r="A16" s="8" t="n"/>
-      <c r="B16" s="8" t="n"/>
+      <c r="D12" s="7" t="inlineStr">
+        <is>
+          <t>05/16/24</t>
+        </is>
+      </c>
+    </row>
+    <row r="13" ht="14.25" customHeight="1" s="8">
+      <c r="A13" s="7" t="inlineStr">
+        <is>
+          <t>A00223332</t>
+        </is>
+      </c>
+      <c r="B13" s="7" t="inlineStr">
+        <is>
+          <t>Nolan Finch</t>
+        </is>
+      </c>
+      <c r="C13" s="10" t="inlineStr">
+        <is>
+          <t>1130:N30</t>
+        </is>
+      </c>
+      <c r="D13" s="7" t="inlineStr">
+        <is>
+          <t>05/29/24</t>
+        </is>
+      </c>
+    </row>
+    <row r="14" ht="14.25" customHeight="1" s="8"/>
+    <row r="15" ht="14.25" customHeight="1" s="8"/>
+    <row r="16" ht="14.25" customHeight="1" s="8">
       <c r="C16" s="10" t="n"/>
-      <c r="D16" s="8" t="n"/>
-    </row>
-    <row r="17" ht="14.25" customHeight="1" s="7">
-      <c r="A17" s="8" t="n"/>
-      <c r="B17" s="8" t="n"/>
-      <c r="C17" s="8" t="n"/>
-      <c r="D17" s="8" t="n"/>
-    </row>
-    <row r="18" ht="14.25" customHeight="1" s="7">
-      <c r="A18" s="8" t="n"/>
-      <c r="B18" s="8" t="n"/>
+    </row>
+    <row r="17" ht="14.25" customHeight="1" s="8"/>
+    <row r="18" ht="14.25" customHeight="1" s="8">
       <c r="C18" s="10" t="n"/>
-      <c r="D18" s="8" t="n"/>
-    </row>
-    <row r="19" ht="14.25" customHeight="1" s="7">
-      <c r="A19" s="8" t="n"/>
-      <c r="B19" s="8" t="n"/>
+    </row>
+    <row r="19" ht="14.25" customHeight="1" s="8">
       <c r="C19" s="10" t="n"/>
-      <c r="D19" s="8" t="n"/>
-    </row>
-    <row r="20" ht="14.25" customHeight="1" s="7">
-      <c r="A20" s="8" t="n"/>
-      <c r="B20" s="8" t="n"/>
-      <c r="C20" s="8" t="n"/>
-      <c r="D20" s="8" t="n"/>
-    </row>
-    <row r="21" ht="14.25" customHeight="1" s="7">
-      <c r="A21" s="8" t="n"/>
-      <c r="B21" s="8" t="n"/>
+    </row>
+    <row r="20" ht="14.25" customHeight="1" s="8"/>
+    <row r="21" ht="14.25" customHeight="1" s="8">
       <c r="C21" s="10" t="n"/>
-      <c r="D21" s="8" t="n"/>
-    </row>
-    <row r="22" ht="14.25" customHeight="1" s="7">
-      <c r="A22" s="8" t="n"/>
-      <c r="B22" s="8" t="n"/>
+    </row>
+    <row r="22" ht="14.25" customHeight="1" s="8">
       <c r="C22" s="10" t="n"/>
-      <c r="D22" s="8" t="n"/>
-    </row>
-    <row r="23" ht="14.25" customHeight="1" s="7">
-      <c r="A23" s="8" t="n"/>
-      <c r="B23" s="8" t="n"/>
+    </row>
+    <row r="23" ht="14.25" customHeight="1" s="8">
       <c r="C23" s="10" t="n"/>
-      <c r="D23" s="8" t="n"/>
-    </row>
-    <row r="24" ht="14.25" customHeight="1" s="7">
-      <c r="A24" s="8" t="n"/>
-      <c r="B24" s="8" t="n"/>
+    </row>
+    <row r="24" ht="14.25" customHeight="1" s="8">
       <c r="C24" s="10" t="n"/>
-      <c r="D24" s="8" t="n"/>
-    </row>
-    <row r="25" ht="13.5" customHeight="1" s="7"/>
+    </row>
+    <row r="25" ht="13.5" customHeight="1" s="8"/>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
@@ -874,64 +855,64 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I16" activeCellId="0" sqref="I16"/>
+      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.8046875" defaultRowHeight="14.25" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.83984375" defaultRowHeight="14.25" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
-    <col width="9.56" customWidth="1" style="8" min="1" max="1"/>
-    <col width="12.64" customWidth="1" style="8" min="2" max="2"/>
+    <col width="9.56" customWidth="1" style="7" min="1" max="1"/>
+    <col width="12.64" customWidth="1" style="7" min="2" max="2"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1" s="7">
-      <c r="A1" s="8" t="inlineStr">
+    <row r="1" ht="14.25" customHeight="1" s="8">
+      <c r="A1" s="7" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="B1" s="8" t="inlineStr">
+      <c r="B1" s="7" t="inlineStr">
         <is>
           <t>A Number</t>
         </is>
       </c>
-      <c r="C1" s="8" t="inlineStr">
+      <c r="C1" s="7" t="inlineStr">
         <is>
           <t>Testing</t>
         </is>
       </c>
-      <c r="D1" s="8" t="inlineStr">
+      <c r="D1" s="7" t="inlineStr">
         <is>
           <t>Course</t>
         </is>
       </c>
-      <c r="E1" s="8" t="inlineStr">
+      <c r="E1" s="7" t="inlineStr">
         <is>
           <t>Section</t>
         </is>
       </c>
-      <c r="F1" s="8" t="inlineStr">
+      <c r="F1" s="7" t="inlineStr">
         <is>
           <t>Calc #</t>
         </is>
       </c>
-      <c r="G1" s="8" t="inlineStr">
+      <c r="G1" s="7" t="inlineStr">
         <is>
           <t>Time In</t>
         </is>
       </c>
-      <c r="H1" s="8" t="inlineStr">
+      <c r="H1" s="7" t="inlineStr">
         <is>
           <t>Time Out</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="13.5" customHeight="1" s="7">
+    <row r="2" ht="13.5" customHeight="1" s="8">
       <c r="A2" s="11" t="inlineStr">
         <is>
-          <t>06/25/24</t>
-        </is>
-      </c>
-      <c r="B2" s="8" t="inlineStr">
+          <t>03/08/24</t>
+        </is>
+      </c>
+      <c r="B2" s="7" t="inlineStr">
         <is>
           <t>A00444555</t>
         </is>
@@ -940,7 +921,7 @@
         <f>TRUE()</f>
         <v/>
       </c>
-      <c r="D2" s="8" t="inlineStr">
+      <c r="D2" s="7" t="inlineStr">
         <is>
           <t>1910</t>
         </is>
@@ -951,7 +932,7 @@
 </t>
         </is>
       </c>
-      <c r="F2" s="8" t="n">
+      <c r="F2" s="7" t="n">
         <v>1</v>
       </c>
       <c r="G2" s="12" t="inlineStr">
@@ -965,13 +946,13 @@
         </is>
       </c>
     </row>
-    <row r="3" ht="13.5" customHeight="1" s="7">
+    <row r="3" ht="13.5" customHeight="1" s="8">
       <c r="A3" s="11" t="inlineStr">
         <is>
-          <t>06/25/24</t>
-        </is>
-      </c>
-      <c r="B3" s="8" t="inlineStr">
+          <t>03/11/24</t>
+        </is>
+      </c>
+      <c r="B3" s="7" t="inlineStr">
         <is>
           <t>A00404303</t>
         </is>
@@ -980,7 +961,7 @@
         <f>TRUE()</f>
         <v/>
       </c>
-      <c r="D3" s="8" t="inlineStr">
+      <c r="D3" s="7" t="inlineStr">
         <is>
           <t>1130</t>
         </is>
@@ -991,7 +972,7 @@
 </t>
         </is>
       </c>
-      <c r="F3" s="8" t="n">
+      <c r="F3" s="7" t="n">
         <v>5</v>
       </c>
       <c r="G3" s="12" t="inlineStr">
@@ -1005,13 +986,13 @@
         </is>
       </c>
     </row>
-    <row r="4" ht="13.5" customHeight="1" s="7">
+    <row r="4" ht="13.5" customHeight="1" s="8">
       <c r="A4" s="11" t="inlineStr">
         <is>
-          <t>06/25/24</t>
-        </is>
-      </c>
-      <c r="B4" s="8" t="inlineStr">
+          <t>04/05/24</t>
+        </is>
+      </c>
+      <c r="B4" s="7" t="inlineStr">
         <is>
           <t>A00909111</t>
         </is>
@@ -1020,7 +1001,7 @@
         <f>FALSE()</f>
         <v/>
       </c>
-      <c r="D4" s="8" t="inlineStr">
+      <c r="D4" s="7" t="inlineStr">
         <is>
           <t>1920</t>
         </is>
@@ -1031,7 +1012,7 @@
 </t>
         </is>
       </c>
-      <c r="F4" s="8" t="n">
+      <c r="F4" s="7" t="n">
         <v>0</v>
       </c>
       <c r="G4" s="12" t="inlineStr">
@@ -1039,19 +1020,19 @@
           <t>14:12</t>
         </is>
       </c>
-      <c r="H4" s="8" t="inlineStr">
+      <c r="H4" s="7" t="inlineStr">
         <is>
           <t>15:53</t>
         </is>
       </c>
     </row>
-    <row r="5" ht="13.5" customHeight="1" s="7">
+    <row r="5" ht="13.5" customHeight="1" s="8">
       <c r="A5" s="11" t="inlineStr">
         <is>
-          <t>06/25/24</t>
-        </is>
-      </c>
-      <c r="B5" s="8" t="inlineStr">
+          <t>04/07/24</t>
+        </is>
+      </c>
+      <c r="B5" s="7" t="inlineStr">
         <is>
           <t>A00898989</t>
         </is>
@@ -1060,17 +1041,17 @@
         <f>TRUE()</f>
         <v/>
       </c>
-      <c r="D5" s="8" t="inlineStr">
+      <c r="D5" s="7" t="inlineStr">
         <is>
           <t>1710</t>
         </is>
       </c>
-      <c r="E5" s="8" t="inlineStr">
+      <c r="E5" s="7" t="inlineStr">
         <is>
           <t>N35</t>
         </is>
       </c>
-      <c r="F5" s="8" t="n">
+      <c r="F5" s="7" t="n">
         <v>12</v>
       </c>
       <c r="G5" s="12" t="inlineStr">
@@ -1078,19 +1059,19 @@
           <t>14:50</t>
         </is>
       </c>
-      <c r="H5" s="8" t="inlineStr">
+      <c r="H5" s="7" t="inlineStr">
         <is>
           <t>16:03</t>
         </is>
       </c>
     </row>
-    <row r="6" ht="13.5" customHeight="1" s="7">
+    <row r="6" ht="13.5" customHeight="1" s="8">
       <c r="A6" s="11" t="inlineStr">
         <is>
-          <t>06/25/24</t>
-        </is>
-      </c>
-      <c r="B6" s="8" t="inlineStr">
+          <t>04/07/24</t>
+        </is>
+      </c>
+      <c r="B6" s="7" t="inlineStr">
         <is>
           <t>A00242424</t>
         </is>
@@ -1099,17 +1080,17 @@
         <f>TRUE()</f>
         <v/>
       </c>
-      <c r="D6" s="8" t="inlineStr">
+      <c r="D6" s="7" t="inlineStr">
         <is>
           <t>2010</t>
         </is>
       </c>
-      <c r="E6" s="8" t="inlineStr">
+      <c r="E6" s="7" t="inlineStr">
         <is>
           <t>N30</t>
         </is>
       </c>
-      <c r="F6" s="8" t="n">
+      <c r="F6" s="7" t="n">
         <v>1</v>
       </c>
       <c r="G6" s="12" t="inlineStr">
@@ -1123,13 +1104,13 @@
         </is>
       </c>
     </row>
-    <row r="7" ht="13.5" customHeight="1" s="7">
+    <row r="7" ht="13.5" customHeight="1" s="8">
       <c r="A7" s="11" t="inlineStr">
         <is>
-          <t>06/25/24</t>
-        </is>
-      </c>
-      <c r="B7" s="8" t="inlineStr">
+          <t>04/10/24</t>
+        </is>
+      </c>
+      <c r="B7" s="7" t="inlineStr">
         <is>
           <t>A00444555</t>
         </is>
@@ -1138,17 +1119,17 @@
         <f>TRUE()</f>
         <v/>
       </c>
-      <c r="D7" s="8" t="inlineStr">
+      <c r="D7" s="7" t="inlineStr">
         <is>
           <t>1910</t>
         </is>
       </c>
-      <c r="E7" s="8" t="inlineStr">
+      <c r="E7" s="7" t="inlineStr">
         <is>
           <t>N35</t>
         </is>
       </c>
-      <c r="F7" s="8" t="n">
+      <c r="F7" s="7" t="n">
         <v>12</v>
       </c>
       <c r="G7" s="12" t="inlineStr">
@@ -1156,19 +1137,19 @@
           <t>14:51</t>
         </is>
       </c>
-      <c r="H7" s="8" t="inlineStr">
+      <c r="H7" s="7" t="inlineStr">
         <is>
           <t>15:56</t>
         </is>
       </c>
     </row>
-    <row r="8" ht="13.5" customHeight="1" s="7">
+    <row r="8" ht="13.5" customHeight="1" s="8">
       <c r="A8" s="11" t="inlineStr">
         <is>
-          <t>06/25/24</t>
-        </is>
-      </c>
-      <c r="B8" s="8" t="inlineStr">
+          <t>04/15/24</t>
+        </is>
+      </c>
+      <c r="B8" s="7" t="inlineStr">
         <is>
           <t>A00123456</t>
         </is>
@@ -1177,17 +1158,17 @@
         <f>FALSE()</f>
         <v/>
       </c>
-      <c r="D8" s="8" t="inlineStr">
+      <c r="D8" s="7" t="inlineStr">
         <is>
           <t>2110</t>
         </is>
       </c>
-      <c r="E8" s="8" t="inlineStr">
+      <c r="E8" s="7" t="inlineStr">
         <is>
           <t>N30</t>
         </is>
       </c>
-      <c r="F8" s="8" t="n">
+      <c r="F8" s="7" t="n">
         <v>0</v>
       </c>
       <c r="G8" s="12" t="inlineStr">
@@ -1195,19 +1176,19 @@
           <t>14:52</t>
         </is>
       </c>
-      <c r="H8" s="8" t="inlineStr">
+      <c r="H8" s="7" t="inlineStr">
         <is>
           <t>16:18</t>
         </is>
       </c>
     </row>
-    <row r="9" ht="13.5" customHeight="1" s="7">
+    <row r="9" ht="13.5" customHeight="1" s="8">
       <c r="A9" s="11" t="inlineStr">
         <is>
-          <t>06/25/24</t>
-        </is>
-      </c>
-      <c r="B9" s="8" t="inlineStr">
+          <t>04/17/24</t>
+        </is>
+      </c>
+      <c r="B9" s="7" t="inlineStr">
         <is>
           <t>A00654321</t>
         </is>
@@ -1216,17 +1197,17 @@
         <f>TRUE()</f>
         <v/>
       </c>
-      <c r="D9" s="8" t="inlineStr">
+      <c r="D9" s="7" t="inlineStr">
         <is>
           <t>1910</t>
         </is>
       </c>
-      <c r="E9" s="8" t="inlineStr">
+      <c r="E9" s="7" t="inlineStr">
         <is>
           <t>N35</t>
         </is>
       </c>
-      <c r="F9" s="8" t="n">
+      <c r="F9" s="7" t="n">
         <v>20</v>
       </c>
       <c r="G9" s="12" t="inlineStr">
@@ -1234,19 +1215,19 @@
           <t>14:53</t>
         </is>
       </c>
-      <c r="H9" s="8" t="inlineStr">
+      <c r="H9" s="7" t="inlineStr">
         <is>
           <t>16:17</t>
         </is>
       </c>
     </row>
-    <row r="10" ht="13.5" customHeight="1" s="7">
+    <row r="10" ht="13.5" customHeight="1" s="8">
       <c r="A10" s="11" t="inlineStr">
         <is>
-          <t>06/27/24</t>
-        </is>
-      </c>
-      <c r="B10" s="8" t="inlineStr">
+          <t>04/17/24</t>
+        </is>
+      </c>
+      <c r="B10" s="7" t="inlineStr">
         <is>
           <t>A00444555</t>
         </is>
@@ -1255,17 +1236,17 @@
         <f>TRUE()</f>
         <v/>
       </c>
-      <c r="D10" s="8" t="inlineStr">
+      <c r="D10" s="7" t="inlineStr">
         <is>
           <t>1910</t>
         </is>
       </c>
-      <c r="E10" s="8" t="inlineStr">
+      <c r="E10" s="7" t="inlineStr">
         <is>
           <t>N35</t>
         </is>
       </c>
-      <c r="F10" s="8" t="n">
+      <c r="F10" s="7" t="n">
         <v>0</v>
       </c>
       <c r="G10" s="12" t="inlineStr">
@@ -1273,19 +1254,19 @@
           <t>13:17</t>
         </is>
       </c>
-      <c r="H10" s="8" t="inlineStr">
+      <c r="H10" s="7" t="inlineStr">
         <is>
           <t>17:13</t>
         </is>
       </c>
     </row>
-    <row r="11" ht="13.5" customHeight="1" s="7">
+    <row r="11" ht="13.5" customHeight="1" s="8">
       <c r="A11" s="11" t="inlineStr">
         <is>
-          <t>06/27/24</t>
-        </is>
-      </c>
-      <c r="B11" s="8" t="inlineStr">
+          <t>05/02/24</t>
+        </is>
+      </c>
+      <c r="B11" s="7" t="inlineStr">
         <is>
           <t>A00345345</t>
         </is>
@@ -1294,17 +1275,17 @@
         <f>TRUE()</f>
         <v/>
       </c>
-      <c r="D11" s="8" t="inlineStr">
+      <c r="D11" s="7" t="inlineStr">
         <is>
           <t>1920</t>
         </is>
       </c>
-      <c r="E11" s="8" t="inlineStr">
+      <c r="E11" s="7" t="inlineStr">
         <is>
           <t>N30</t>
         </is>
       </c>
-      <c r="F11" s="8" t="n">
+      <c r="F11" s="7" t="n">
         <v>4</v>
       </c>
       <c r="G11" s="12" t="inlineStr">
@@ -1312,19 +1293,19 @@
           <t>16:49</t>
         </is>
       </c>
-      <c r="H11" s="8" t="inlineStr">
+      <c r="H11" s="7" t="inlineStr">
         <is>
           <t>17:13</t>
         </is>
       </c>
     </row>
-    <row r="12" ht="13.5" customHeight="1" s="7">
+    <row r="12" ht="13.5" customHeight="1" s="8">
       <c r="A12" s="11" t="inlineStr">
         <is>
-          <t>06/27/24</t>
-        </is>
-      </c>
-      <c r="B12" s="8" t="inlineStr">
+          <t>05/10/24</t>
+        </is>
+      </c>
+      <c r="B12" s="7" t="inlineStr">
         <is>
           <t>A00456123</t>
         </is>
@@ -1333,17 +1314,17 @@
         <f>FALSE()</f>
         <v/>
       </c>
-      <c r="D12" s="8" t="inlineStr">
+      <c r="D12" s="7" t="inlineStr">
         <is>
           <t>1920</t>
         </is>
       </c>
-      <c r="E12" s="8" t="inlineStr">
+      <c r="E12" s="7" t="inlineStr">
         <is>
           <t>N30</t>
         </is>
       </c>
-      <c r="F12" s="8" t="n">
+      <c r="F12" s="7" t="n">
         <v>19</v>
       </c>
       <c r="G12" s="12" t="inlineStr">
@@ -1351,37 +1332,38 @@
           <t>16:51</t>
         </is>
       </c>
-      <c r="H12" s="8" t="inlineStr">
+      <c r="H12" s="7" t="inlineStr">
         <is>
           <t>17:14</t>
         </is>
       </c>
     </row>
-    <row r="13" ht="13.5" customHeight="1" s="7">
+    <row r="13" ht="13.5" customHeight="1" s="8">
       <c r="A13" s="11" t="inlineStr">
         <is>
-          <t>06/27/24</t>
-        </is>
-      </c>
-      <c r="B13" s="8" t="inlineStr">
+          <t>05/10/24</t>
+        </is>
+      </c>
+      <c r="B13" s="7" t="inlineStr">
         <is>
           <t>A00242424</t>
         </is>
       </c>
-      <c r="C13" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D13" s="8" t="inlineStr">
+      <c r="C13" s="9">
+        <f>FALSE()</f>
+        <v/>
+      </c>
+      <c r="D13" s="7" t="inlineStr">
         <is>
           <t>2010</t>
         </is>
       </c>
-      <c r="E13" s="8" t="inlineStr">
+      <c r="E13" s="7" t="inlineStr">
         <is>
           <t>N30</t>
         </is>
       </c>
-      <c r="F13" s="8" t="n">
+      <c r="F13" s="7" t="n">
         <v>14</v>
       </c>
       <c r="G13" s="12" t="inlineStr">
@@ -1389,123 +1371,126 @@
           <t>17:29</t>
         </is>
       </c>
-      <c r="H13" s="8" t="inlineStr">
-        <is>
-          <t>17:29</t>
-        </is>
-      </c>
-    </row>
-    <row r="14" ht="13.5" customHeight="1" s="7">
+      <c r="H13" s="7" t="inlineStr">
+        <is>
+          <t>18:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="14" ht="13.5" customHeight="1" s="8">
       <c r="A14" s="11" t="inlineStr">
         <is>
-          <t>06/28/24</t>
-        </is>
-      </c>
-      <c r="B14" s="8" t="inlineStr">
+          <t>05/16/24</t>
+        </is>
+      </c>
+      <c r="B14" s="7" t="inlineStr">
         <is>
           <t>A00999111</t>
         </is>
       </c>
-      <c r="C14" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D14" s="8" t="inlineStr">
+      <c r="C14" s="9">
+        <f>TRUE()</f>
+        <v/>
+      </c>
+      <c r="D14" s="7" t="inlineStr">
         <is>
           <t>1720</t>
         </is>
       </c>
-      <c r="E14" s="8" t="inlineStr">
+      <c r="E14" s="7" t="inlineStr">
         <is>
           <t>N35</t>
         </is>
       </c>
-      <c r="F14" s="8" t="n">
+      <c r="F14" s="7" t="n">
         <v>13</v>
       </c>
       <c r="G14" s="12" t="inlineStr">
         <is>
-          <t>18:29</t>
-        </is>
-      </c>
-      <c r="H14" s="8" t="inlineStr">
-        <is>
-          <t>18:29</t>
-        </is>
-      </c>
-    </row>
-    <row r="15" ht="13.5" customHeight="1" s="7">
+          <t>12:29</t>
+        </is>
+      </c>
+      <c r="H14" s="7" t="inlineStr">
+        <is>
+          <t>13:51</t>
+        </is>
+      </c>
+    </row>
+    <row r="15" ht="13.5" customHeight="1" s="8">
       <c r="A15" s="11" t="inlineStr">
         <is>
-          <t>06/28/24</t>
-        </is>
-      </c>
-      <c r="B15" s="8" t="inlineStr">
+          <t>05/16/24</t>
+        </is>
+      </c>
+      <c r="B15" s="7" t="inlineStr">
         <is>
           <t>A00663224</t>
         </is>
       </c>
-      <c r="C15" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D15" s="8" t="inlineStr">
+      <c r="C15" s="9">
+        <f>TRUE()</f>
+        <v/>
+      </c>
+      <c r="D15" s="7" t="inlineStr">
         <is>
           <t>2110</t>
         </is>
       </c>
-      <c r="E15" s="8" t="inlineStr">
+      <c r="E15" s="7" t="inlineStr">
         <is>
           <t>N30</t>
         </is>
       </c>
-      <c r="F15" s="8" t="n">
+      <c r="F15" s="7" t="n">
         <v>21</v>
       </c>
-      <c r="G15" s="8" t="inlineStr">
-        <is>
-          <t>23:49</t>
-        </is>
-      </c>
-      <c r="H15" s="8" t="inlineStr">
-        <is>
-          <t>23:49</t>
-        </is>
-      </c>
-    </row>
-    <row r="16" ht="13.5" customHeight="1" s="7">
-      <c r="A16" s="8" t="inlineStr">
-        <is>
-          <t>06/29/24</t>
-        </is>
-      </c>
-      <c r="B16" s="8" t="inlineStr">
-        <is>
-          <t>A00999111</t>
-        </is>
-      </c>
-      <c r="C16" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D16" s="8" t="inlineStr">
-        <is>
-          <t>1720</t>
-        </is>
-      </c>
-      <c r="E16" s="8" t="inlineStr">
-        <is>
-          <t>N35</t>
-        </is>
-      </c>
-      <c r="F16" s="8" t="n">
-        <v>5</v>
-      </c>
-      <c r="G16" s="8" t="inlineStr">
-        <is>
-          <t>01:29</t>
-        </is>
-      </c>
-      <c r="H16" s="8" t="inlineStr">
-        <is>
-          <t>01:29</t>
+      <c r="G15" s="7" t="inlineStr">
+        <is>
+          <t>14:49</t>
+        </is>
+      </c>
+      <c r="H15" s="7" t="inlineStr">
+        <is>
+          <t>15:35</t>
+        </is>
+      </c>
+    </row>
+    <row r="16" ht="13.5" customHeight="1" s="8">
+      <c r="A16" s="7" t="inlineStr">
+        <is>
+          <t>05/29/24</t>
+        </is>
+      </c>
+      <c r="B16" s="7" t="inlineStr">
+        <is>
+          <t>A00223332</t>
+        </is>
+      </c>
+      <c r="C16" s="9">
+        <f>FALSE()</f>
+        <v/>
+      </c>
+      <c r="D16" s="7" t="inlineStr">
+        <is>
+          <t>1130</t>
+        </is>
+      </c>
+      <c r="E16" s="7" t="inlineStr">
+        <is>
+          <t>N30</t>
+        </is>
+      </c>
+      <c r="F16" s="7" t="n">
+        <v>55</v>
+      </c>
+      <c r="G16" s="7" t="inlineStr">
+        <is>
+          <t>14:53</t>
+        </is>
+      </c>
+      <c r="H16" s="13" t="inlineStr">
+        <is>
+          <t>18:13</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed file i/o bug
</commit_message>
<xml_diff>
--- a/data/Visitors.xlsx
+++ b/data/Visitors.xlsx
@@ -813,7 +813,28 @@
         </is>
       </c>
     </row>
-    <row r="14" ht="14.25" customHeight="1" s="8"/>
+    <row r="14" ht="14.25" customHeight="1" s="8">
+      <c r="A14" s="7" t="inlineStr">
+        <is>
+          <t>A00887554</t>
+        </is>
+      </c>
+      <c r="B14" s="7" t="inlineStr">
+        <is>
+          <t>Sam Seder</t>
+        </is>
+      </c>
+      <c r="C14" s="7" t="inlineStr">
+        <is>
+          <t>1920:N30</t>
+        </is>
+      </c>
+      <c r="D14" s="7" t="inlineStr">
+        <is>
+          <t>09/08/24</t>
+        </is>
+      </c>
+    </row>
     <row r="15" ht="14.25" customHeight="1" s="8"/>
     <row r="16" ht="14.25" customHeight="1" s="8">
       <c r="C16" s="10" t="n"/>
@@ -1458,21 +1479,20 @@
     <row r="16" ht="13.5" customHeight="1" s="8">
       <c r="A16" s="7" t="inlineStr">
         <is>
-          <t>05/29/24</t>
+          <t>09/08/24</t>
         </is>
       </c>
       <c r="B16" s="7" t="inlineStr">
         <is>
-          <t>A00223332</t>
-        </is>
-      </c>
-      <c r="C16" s="9">
-        <f>FALSE()</f>
-        <v/>
+          <t>A00887554</t>
+        </is>
+      </c>
+      <c r="C16" s="9" t="b">
+        <v>1</v>
       </c>
       <c r="D16" s="7" t="inlineStr">
         <is>
-          <t>1130</t>
+          <t>1920</t>
         </is>
       </c>
       <c r="E16" s="7" t="inlineStr">
@@ -1481,16 +1501,16 @@
         </is>
       </c>
       <c r="F16" s="7" t="n">
-        <v>55</v>
+        <v>13</v>
       </c>
       <c r="G16" s="7" t="inlineStr">
         <is>
-          <t>14:53</t>
+          <t>18:39</t>
         </is>
       </c>
       <c r="H16" s="13" t="inlineStr">
         <is>
-          <t>18:13</t>
+          <t>18:39</t>
         </is>
       </c>
     </row>

</xml_diff>